<commit_message>
Changing Figure 1 and results table
</commit_message>
<xml_diff>
--- a/Years - Causess + Gender Descriptive Statistics/Years - Causes + Gender Results.xlsx
+++ b/Years - Causess + Gender Descriptive Statistics/Years - Causes + Gender Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/38afa0e73f251f50/Рабочий стол/Mortality-rate-second/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/38afa0e73f251f50/Рабочий стол/Mortality-rate-second/Years - Causess ^M Gender Descriptive Statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="6" documentId="11_AD4DF75460589B3ACB728475575E616C5ADEDD96" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{822A08EA-1595-4C6A-810B-F5C2022767E7}"/>
@@ -461,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="66" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modified figure 1 & 2
</commit_message>
<xml_diff>
--- a/Years - Causess + Gender Descriptive Statistics/Years - Causes + Gender Results.xlsx
+++ b/Years - Causess + Gender Descriptive Statistics/Years - Causes + Gender Results.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/38afa0e73f251f50/Рабочий стол/Mortality-rate-second/Years - Causess ^M Gender Descriptive Statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_AD4DF75460589B3ACB728475575E616C5ADEDD96" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{822A08EA-1595-4C6A-810B-F5C2022767E7}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{CFFA23FB-FCBF-48A9-B9C6-C4CC9876BE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C5FFF2D-D5C5-4CA8-AA7D-C78B708613B8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId3"/>
+  </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,9 +38,6 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Obseration</t>
-  </si>
-  <si>
     <t>Switzerland</t>
   </si>
   <si>
@@ -51,24 +53,12 @@
     <t>Rapid increase in death rate from 1980s. Men have higher mortality rates.</t>
   </si>
   <si>
-    <t>Until 1990, mortality trends in both Switzerland and Japan appeared to be comparable. However, a divergence occurred thereafter, with Switzerland experiencing a decline in mortality while Japan witnessed an increase.</t>
-  </si>
-  <si>
     <t>A significant decline in mortality rates occurred around 1995.</t>
   </si>
   <si>
-    <t>In Japan, there was a notable increase in mortality rates after the year 2000, accompanied by isolated spike in 2011.</t>
-  </si>
-  <si>
-    <t>Non-communicable diseases stand as the leading cause, exerting the most significant influence on the primary mortality trends. Proportionally, they constitute the largest share of all mortality, establishing the prevailing trend. The reason behind the upswing in statistics is challenging to conjecture, given the multitude of factors at play.</t>
-  </si>
-  <si>
     <t>There was an outbreak of tuberculosis from 1975 to 2000.</t>
   </si>
   <si>
-    <t>In Japan, something appears to have transpired concerning low respiratory diseases, as they specifically underpin the surge in statistics.</t>
-  </si>
-  <si>
     <t>Among other injury types, notably poisonings and falls distinguished, for which a substantial decline in mortality was observed.</t>
   </si>
   <si>
@@ -81,7 +71,25 @@
     <t>Hypothetical explanation</t>
   </si>
   <si>
-    <t>In 2011, the strongest earthquake in history of Japan transpired followed by tsunami, where individuals predominantly succumbed to injuries. Furthermore, if we scrutinize the chart for natural disasters, this pattern becomes evident for both 1995 and 2011, as earthquakes were prevalent in both years.  Moreover, the Fukushima tragedy was due to the earthquake in 2011 , which also played a huge role in increase in the number of deaths from injuries.</t>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>In Japan, something appears to have provoked the spread of deadly low respiratory diseases, as they specifically underpin the surge in statistics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Non-communicable diseases are the primary cause, significantly influencing mortality trends. They constitute the largest share of all deaths, setting the prevailing trend. The increase in statistics is challenging to explain due to numerous contributing factors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Until 1990, mortality trends in Switzerland and Japan seemed similar. However, a shift occurred afterward, with Switzerland seeing a decrease in mortality while Japan observed an increase.</t>
+  </si>
+  <si>
+    <t>In Japan, there was a notable increase in mortality rates after the year 1990, accompanied by isolated spikes in 2011 and 1995.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+In 2011, Japan experienced its strongest earthquake, followed by a tsunami where many individuals suffered fatal injuries. Furthermore, the Fukushima tragedy in 2011, caused by the earthquake, played a significant role in the increase in the number of deaths from injuries. Additionally, the charts indicate a mortality rate spike in 1995, attributed to an earthquake in that year.</t>
   </si>
 </sst>
 </file>
@@ -112,7 +120,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +133,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -149,23 +163,125 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -173,10 +289,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -194,6 +325,107 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Варвара" refreshedDate="45317.637006481484" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="6" xr:uid="{C1D2F219-A555-43AF-9106-9F273BBC3443}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:D7" sheet="Лист1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Cause" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Country" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Obseration" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Hypothetical explanation" numFmtId="0">
+      <sharedItems containsBlank="1" longText="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="6">
+  <r>
+    <s v="Noncommunicable diseases (+Malignant neoplasms)"/>
+    <s v="Switzerland"/>
+    <s v="Trend of a slow decline in mortality. After 2000, the mortality rate of women in Switzerland surpassed that of men."/>
+    <s v="Non-communicable diseases stand as the leading cause, exerting the most significant influence on the primary mortality trends. Proportionally, they constitute the largest share of all mortality, establishing the prevailing trend. The reason behind the upswing in statistics is challenging to conjecture, given the multitude of factors at play."/>
+  </r>
+  <r>
+    <m/>
+    <s v="Japan"/>
+    <s v="Rapid increase in death rate from 1980s. Men have higher mortality rates."/>
+    <m/>
+  </r>
+  <r>
+    <s v="Communicable, maternal, perinatal and nutritional conditions"/>
+    <s v="Switzerland"/>
+    <s v="Until 1990, mortality trends in both Switzerland and Japan appeared to be comparable. However, a divergence occurred thereafter, with Switzerland experiencing a decline in mortality while Japan witnessed an increase."/>
+    <s v="There was an outbreak of tuberculosis from 1975 to 2000."/>
+  </r>
+  <r>
+    <m/>
+    <s v="Japan"/>
+    <m/>
+    <s v="In Japan, something appears to have transpired concerning low respiratory diseases, as they specifically underpin the surge in statistics."/>
+  </r>
+  <r>
+    <s v="Injuries"/>
+    <s v="Switzerland"/>
+    <s v="A significant decline in mortality rates occurred around 1995."/>
+    <s v="Among other injury types, notably poisonings and falls distinguished, for which a substantial decline in mortality was observed."/>
+  </r>
+  <r>
+    <m/>
+    <s v="Japan"/>
+    <s v="In Japan, there was a notable increase in mortality rates after the year 2000, accompanied by isolated spike in 2011."/>
+    <s v="In 2011, the strongest earthquake in history of Japan transpired followed by tsunami, where individuals predominantly succumbed to injuries. Furthermore, if we scrutinize the chart for natural disasters, this pattern becomes evident for both 1995 and 2011, as earthquakes were prevalent in both years.  Moreover, the Fukushima tragedy was due to the earthquake in 2011 , which also played a huge role in increase in the number of deaths from injuries."/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{836C193C-753C-4EC2-9781-96B0FA0566F0}" name="Сводная таблица1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,107 +690,212 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99597E6-7222-4A85-B117-8BF95C523D05}">
+  <dimension ref="A3:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="66" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.6328125" customWidth="1"/>
     <col min="2" max="2" width="15.6328125" customWidth="1"/>
-    <col min="3" max="3" width="41.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.6328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="8"/>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="145" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="16" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>